<commit_message>
update database source files
</commit_message>
<xml_diff>
--- a/design/data/Australian Food Composition Database/Release 2 - Nutrient file(Pete).xlsx
+++ b/design/data/Australian Food Composition Database/Release 2 - Nutrient file(Pete).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peteburquette/Documents/Code/Portfolio/glycemic_limit_native/design/data/Australian Food Composition Database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peteburquette/Documents/Code/Portfolio/KetoLimit/design/data/Australian Food Composition Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA943D29-A73C-B944-A65B-DA6C243D55AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828B090A-3183-0645-AA4D-D5F7FB46C9E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="5740" windowWidth="27000" windowHeight="22360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="4200" windowWidth="27000" windowHeight="22360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All solids &amp; liquids per 100g" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="3330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="3331">
   <si>
     <t>F002258</t>
   </si>
@@ -10013,6 +10013,9 @@
   </si>
   <si>
     <t>saturatedFat</t>
+  </si>
+  <si>
+    <t>-1</t>
   </si>
 </sst>
 </file>
@@ -10621,10 +10624,10 @@
   <dimension ref="A1:O1617"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D227" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B250" sqref="B250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13515,7 +13518,9 @@
       <c r="A62" s="27" t="s">
         <v>3032</v>
       </c>
-      <c r="B62" s="24"/>
+      <c r="B62" s="24" t="s">
+        <v>3330</v>
+      </c>
       <c r="C62" s="1" t="s">
         <v>3033</v>
       </c>
@@ -22302,7 +22307,9 @@
       <c r="A249" s="27" t="s">
         <v>3075</v>
       </c>
-      <c r="B249" s="24"/>
+      <c r="B249" s="24" t="s">
+        <v>3330</v>
+      </c>
       <c r="C249" s="1" t="s">
         <v>3076</v>
       </c>

</xml_diff>